<commit_message>
Just to ensure :wink:
</commit_message>
<xml_diff>
--- a/Hints/Sima Report Helper.xlsx
+++ b/Hints/Sima Report Helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Hints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C557770E-BE80-43A3-8628-459E0C147724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B391C771-0F09-4984-87EC-AA00DEA21772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FEC91C08-D9C3-4A52-9334-DA230FE3FFEF}"/>
   </bookViews>
@@ -422,6 +422,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,34 +461,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -787,7 +787,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,27 +806,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="14" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -847,25 +847,25 @@
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="14">
         <v>1</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="21">
+      <c r="J2" s="14">
         <v>1</v>
       </c>
-      <c r="K2" s="22">
+      <c r="K2" s="15">
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="17">
         <v>1</v>
       </c>
     </row>
@@ -888,25 +888,25 @@
       <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="14">
         <v>3</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="15">
         <v>2</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="21">
+      <c r="J3" s="14">
         <v>21</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="15">
         <v>2</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="24">
+      <c r="M3" s="17">
         <v>31</v>
       </c>
     </row>
@@ -929,21 +929,21 @@
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="14">
         <v>4</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="22">
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="15">
         <v>3</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="17">
         <v>32</v>
       </c>
     </row>
@@ -966,25 +966,25 @@
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="14">
         <v>5</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="15">
         <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="14">
         <v>1</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="15">
         <v>4</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="17">
         <v>33</v>
       </c>
     </row>
@@ -1007,25 +1007,25 @@
       <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="14">
         <v>6</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="15">
         <v>2</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="14">
         <v>22</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6" s="16">
         <v>5</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="18">
         <v>34</v>
       </c>
     </row>
@@ -1048,23 +1048,23 @@
       <c r="F7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="14">
         <v>7</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="15">
         <v>3</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="14">
         <v>23</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1085,25 +1085,25 @@
       <c r="F8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="14">
         <v>8</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="15">
         <v>4</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="14">
         <v>24</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="15">
         <v>1</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1126,21 +1126,21 @@
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="14">
         <v>9</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="22">
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="15">
         <v>2</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="17">
         <v>35</v>
       </c>
     </row>
@@ -1163,16 +1163,16 @@
       <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="14">
         <v>10</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="15">
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1195,16 +1195,16 @@
       <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="14">
         <v>11</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="15">
         <v>2</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="14">
         <v>25</v>
       </c>
     </row>
@@ -1227,16 +1227,16 @@
       <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="14">
         <v>12</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="15">
         <v>3</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="14">
         <v>26</v>
       </c>
     </row>
@@ -1259,16 +1259,16 @@
       <c r="F13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="14">
         <v>13</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="15">
         <v>4</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="14">
         <v>24</v>
       </c>
     </row>
@@ -1291,16 +1291,16 @@
       <c r="F14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="14">
         <v>14</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="15">
         <v>5</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="14">
         <v>28</v>
       </c>
     </row>
@@ -1323,16 +1323,16 @@
       <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="14">
         <v>15</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="15">
         <v>6</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="14">
         <v>29</v>
       </c>
     </row>
@@ -1355,16 +1355,16 @@
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="14">
         <v>16</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="15">
         <v>7</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="14">
         <v>30</v>
       </c>
     </row>
@@ -1387,7 +1387,7 @@
       <c r="F17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="14">
         <v>17</v>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       <c r="F18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="14">
         <v>18</v>
       </c>
     </row>
@@ -1433,7 +1433,7 @@
       <c r="F19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="14">
         <v>19</v>
       </c>
     </row>
@@ -1448,7 +1448,7 @@
       <c r="F20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="14">
         <v>20</v>
       </c>
     </row>
@@ -1488,18 +1488,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -1514,13 +1514,13 @@
         <v>48</v>
       </c>
       <c r="B3" s="27"/>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="11" t="s">
         <v>29</v>
       </c>
@@ -1534,11 +1534,11 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
       <c r="G4" s="12" t="s">
         <v>31</v>
       </c>
@@ -1550,10 +1550,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="11" t="s">
         <v>45</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>56</v>
       </c>
       <c r="F5" s="27"/>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="19" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1572,14 +1572,14 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="12" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="20" t="s">
         <v>32</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1594,13 +1594,13 @@
         <v>50</v>
       </c>
       <c r="B7" s="27"/>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="11" t="s">
         <v>60</v>
       </c>
@@ -1614,20 +1614,20 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="27"/>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="11" t="s">
         <v>20</v>
       </c>
@@ -1635,19 +1635,19 @@
         <v>58</v>
       </c>
       <c r="F9" s="27"/>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="12" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="20" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1656,13 +1656,13 @@
         <v>52</v>
       </c>
       <c r="B11" s="27"/>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="11" t="s">
         <v>62</v>
       </c>
@@ -1670,27 +1670,27 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="27"/>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="20"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="12" t="s">
         <v>34</v>
       </c>
@@ -1700,19 +1700,25 @@
         <v>54</v>
       </c>
       <c r="B15" s="27"/>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="19" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="20" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A13:B14"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="E7:F8"/>
     <mergeCell ref="E9:F10"/>
     <mergeCell ref="E11:F12"/>
     <mergeCell ref="A3:B4"/>
@@ -1720,12 +1726,6 @@
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="A11:B12"/>
-    <mergeCell ref="A13:B14"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>